<commit_message>
Changes in the cuota calculation and comparison included in the pdf by running report.R again
</commit_message>
<xml_diff>
--- a/results/2023_Summaryplots.xlsx
+++ b/results/2023_Summaryplots.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -88,13 +88,919 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="308">
+  <cellXfs count="610">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
       <alignment wrapText="true"/>
     </xf>
@@ -1022,554 +1928,554 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="157">
+      <c r="A1" t="s" s="459">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="158">
+      <c r="B1" t="s" s="460">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="159">
+      <c r="C1" t="s" s="461">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="160">
+      <c r="D1" t="s" s="462">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="161">
+      <c r="E1" t="s" s="463">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="162">
+      <c r="A2" t="n" s="464">
         <v>1989.0</v>
       </c>
-      <c r="B2" t="n" s="197">
+      <c r="B2" t="n" s="499">
         <v>0.599753235</v>
       </c>
-      <c r="C2" t="n" s="231">
+      <c r="C2" t="n" s="533">
         <v>3516.4692</v>
       </c>
-      <c r="D2" t="n" s="266">
+      <c r="D2" t="n" s="568">
         <v>5319.032</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="163">
+      <c r="A3" t="n" s="465">
         <v>1990.0</v>
       </c>
-      <c r="B3" t="n" s="198">
+      <c r="B3" t="n" s="500">
         <v>1.723236275</v>
       </c>
-      <c r="C3" t="n" s="232">
+      <c r="C3" t="n" s="534">
         <v>4677.8064</v>
       </c>
-      <c r="D3" t="n" s="267">
+      <c r="D3" t="n" s="569">
         <v>6689.548000000001</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="164">
+      <c r="A4" t="n" s="466">
         <v>1991.0</v>
       </c>
-      <c r="B4" t="n" s="199">
+      <c r="B4" t="n" s="501">
         <v>0.750756725</v>
       </c>
-      <c r="C4" t="n" s="233">
+      <c r="C4" t="n" s="535">
         <v>2551.796</v>
       </c>
-      <c r="D4" t="n" s="268">
+      <c r="D4" t="n" s="570">
         <v>3468.7690000000002</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="165">
+      <c r="A5" t="n" s="467">
         <v>1992.0</v>
       </c>
-      <c r="B5" t="n" s="200">
+      <c r="B5" t="n" s="502">
         <v>0.5190028315</v>
       </c>
-      <c r="C5" t="n" s="234">
+      <c r="C5" t="n" s="536">
         <v>2104.656</v>
       </c>
-      <c r="D5" t="n" s="269">
+      <c r="D5" t="n" s="571">
         <v>2191.456</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="166">
+      <c r="A6" t="n" s="468">
         <v>1993.0</v>
       </c>
-      <c r="B6" t="n" s="201">
+      <c r="B6" t="n" s="503">
         <v>1.1252008925</v>
       </c>
-      <c r="C6" t="n" s="235">
+      <c r="C6" t="n" s="537">
         <v>2061.342</v>
       </c>
-      <c r="D6" t="n" s="270">
+      <c r="D6" t="n" s="572">
         <v>3016.8668</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="167">
+      <c r="A7" t="n" s="469">
         <v>1994.0</v>
       </c>
-      <c r="B7" t="n" s="202">
+      <c r="B7" t="n" s="504">
         <v>0.1069586085</v>
       </c>
-      <c r="C7" t="n" s="236">
+      <c r="C7" t="n" s="538">
         <v>1309.0810000000001</v>
       </c>
-      <c r="D7" t="n" s="271">
+      <c r="D7" t="n" s="573">
         <v>555.76974</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="168">
+      <c r="A8" t="n" s="470">
         <v>1995.0</v>
       </c>
-      <c r="B8" t="n" s="203">
+      <c r="B8" t="n" s="505">
         <v>0.1439239215</v>
       </c>
-      <c r="C8" t="n" s="237">
+      <c r="C8" t="n" s="539">
         <v>3987.493</v>
       </c>
-      <c r="D8" t="n" s="272">
+      <c r="D8" t="n" s="574">
         <v>1153.59391</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="169">
+      <c r="A9" t="n" s="471">
         <v>1996.0</v>
       </c>
-      <c r="B9" t="n" s="204">
+      <c r="B9" t="n" s="506">
         <v>0.634217375</v>
       </c>
-      <c r="C9" t="n" s="238">
+      <c r="C9" t="n" s="540">
         <v>10152.73</v>
       </c>
-      <c r="D9" t="n" s="273">
+      <c r="D9" t="n" s="575">
         <v>3001.0653</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="170">
+      <c r="A10" t="n" s="472">
         <v>1997.0</v>
       </c>
-      <c r="B10" t="n" s="205">
+      <c r="B10" t="n" s="507">
         <v>0.9905072225</v>
       </c>
-      <c r="C10" t="n" s="239">
+      <c r="C10" t="n" s="541">
         <v>6394.66</v>
       </c>
-      <c r="D10" t="n" s="274">
+      <c r="D10" t="n" s="576">
         <v>6552.2829</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="171">
+      <c r="A11" t="n" s="473">
         <v>1998.0</v>
       </c>
-      <c r="B11" t="n" s="206">
+      <c r="B11" t="n" s="508">
         <v>1.791055225</v>
       </c>
-      <c r="C11" t="n" s="240">
+      <c r="C11" t="n" s="542">
         <v>7971.91</v>
       </c>
-      <c r="D11" t="n" s="275">
+      <c r="D11" t="n" s="577">
         <v>9258.5939</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="172">
+      <c r="A12" t="n" s="474">
         <v>1999.0</v>
       </c>
-      <c r="B12" t="n" s="207">
+      <c r="B12" t="n" s="509">
         <v>1.2146312424999999</v>
       </c>
-      <c r="C12" t="n" s="241">
+      <c r="C12" t="n" s="543">
         <v>2504.354</v>
       </c>
-      <c r="D12" t="n" s="276">
+      <c r="D12" t="n" s="578">
         <v>3387.3143</v>
       </c>
       <c r="E12"/>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="173">
+      <c r="A13" t="n" s="475">
         <v>2000.0</v>
       </c>
-      <c r="B13" t="n" s="208">
+      <c r="B13" t="n" s="510">
         <v>0.8530399949999999</v>
       </c>
-      <c r="C13" t="n" s="242">
+      <c r="C13" t="n" s="544">
         <v>2777.8909999999996</v>
       </c>
-      <c r="D13" t="n" s="277">
+      <c r="D13" t="n" s="579">
         <v>5545.81998</v>
       </c>
       <c r="E13"/>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="174">
+      <c r="A14" t="n" s="476">
         <v>2001.0</v>
       </c>
-      <c r="B14" t="n" s="209">
+      <c r="B14" t="n" s="511">
         <v>0.8536529350000001</v>
       </c>
-      <c r="C14" t="n" s="243">
+      <c r="C14" t="n" s="545">
         <v>6011.168000000001</v>
       </c>
-      <c r="D14" t="n" s="278">
+      <c r="D14" t="n" s="580">
         <v>9093.53857</v>
       </c>
       <c r="E14"/>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="175">
+      <c r="A15" t="n" s="477">
         <v>2002.0</v>
       </c>
-      <c r="B15" t="n" s="210">
+      <c r="B15" t="n" s="512">
         <v>0.6757601075</v>
       </c>
-      <c r="C15" t="n" s="244">
+      <c r="C15" t="n" s="546">
         <v>6498.434</v>
       </c>
-      <c r="D15" t="n" s="279">
+      <c r="D15" t="n" s="581">
         <v>7081.3061800000005</v>
       </c>
       <c r="E15"/>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="176">
+      <c r="A16" t="n" s="478">
         <v>2003.0</v>
       </c>
-      <c r="B16" t="n" s="211">
+      <c r="B16" t="n" s="513">
         <v>0.70520111</v>
       </c>
-      <c r="C16" t="n" s="245">
+      <c r="C16" t="n" s="547">
         <v>3298.645</v>
       </c>
-      <c r="D16" t="n" s="280">
+      <c r="D16" t="n" s="582">
         <v>4742.13649</v>
       </c>
       <c r="E16"/>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="177">
+      <c r="A17" t="n" s="479">
         <v>2004.0</v>
       </c>
-      <c r="B17" t="n" s="212">
+      <c r="B17" t="n" s="514">
         <v>0.979789955</v>
       </c>
-      <c r="C17" t="n" s="246">
+      <c r="C17" t="n" s="548">
         <v>2501.81</v>
       </c>
-      <c r="D17" t="n" s="281">
+      <c r="D17" t="n" s="583">
         <v>5871.08189</v>
       </c>
       <c r="E17"/>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="178">
+      <c r="A18" t="n" s="480">
         <v>2005.0</v>
       </c>
-      <c r="B18" t="n" s="213">
+      <c r="B18" t="n" s="515">
         <v>0.424277575</v>
       </c>
-      <c r="C18" t="n" s="247">
+      <c r="C18" t="n" s="549">
         <v>3530.361</v>
       </c>
-      <c r="D18" t="n" s="282">
+      <c r="D18" t="n" s="584">
         <v>4744.4489</v>
       </c>
       <c r="E18"/>
     </row>
     <row r="19">
-      <c r="A19" t="n" s="179">
+      <c r="A19" t="n" s="481">
         <v>2006.0</v>
       </c>
-      <c r="B19" t="n" s="214">
+      <c r="B19" t="n" s="516">
         <v>0.3207350095</v>
       </c>
-      <c r="C19" t="n" s="248">
+      <c r="C19" t="n" s="550">
         <v>5572.063</v>
       </c>
-      <c r="D19" t="n" s="283">
+      <c r="D19" t="n" s="585">
         <v>4267.4956999999995</v>
       </c>
       <c r="E19"/>
     </row>
     <row r="20">
-      <c r="A20" t="n" s="180">
+      <c r="A20" t="n" s="482">
         <v>2007.0</v>
       </c>
-      <c r="B20" t="n" s="215">
+      <c r="B20" t="n" s="517">
         <v>0.31151734</v>
       </c>
-      <c r="C20" t="n" s="249">
+      <c r="C20" t="n" s="551">
         <v>9080.94</v>
       </c>
-      <c r="D20" t="n" s="284">
+      <c r="D20" t="n" s="586">
         <v>3517.3119</v>
       </c>
       <c r="E20"/>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="181">
+      <c r="A21" t="n" s="483">
         <v>2008.0</v>
       </c>
-      <c r="B21" t="n" s="216">
+      <c r="B21" t="n" s="518">
         <v>0.37867257</v>
       </c>
-      <c r="C21" t="n" s="250">
+      <c r="C21" t="n" s="552">
         <v>5069.78</v>
       </c>
-      <c r="D21" t="n" s="285">
+      <c r="D21" t="n" s="587">
         <v>3299.5126</v>
       </c>
       <c r="E21"/>
     </row>
     <row r="22">
-      <c r="A22" t="n" s="182">
+      <c r="A22" t="n" s="484">
         <v>2009.0</v>
       </c>
-      <c r="B22" t="n" s="217">
+      <c r="B22" t="n" s="519">
         <v>0.751963528</v>
       </c>
-      <c r="C22" t="n" s="251">
+      <c r="C22" t="n" s="553">
         <v>2844.65</v>
       </c>
-      <c r="D22" t="n" s="286">
+      <c r="D22" t="n" s="588">
         <v>2916.9067</v>
       </c>
       <c r="E22"/>
     </row>
     <row r="23">
-      <c r="A23" t="n" s="183">
+      <c r="A23" t="n" s="485">
         <v>2010.0</v>
       </c>
-      <c r="B23" t="n" s="218">
+      <c r="B23" t="n" s="520">
         <v>0.612094965</v>
       </c>
-      <c r="C23" t="n" s="252">
+      <c r="C23" t="n" s="554">
         <v>1878.51</v>
       </c>
-      <c r="D23" t="n" s="287">
+      <c r="D23" t="n" s="589">
         <v>4820.6776</v>
       </c>
       <c r="E23"/>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="184">
+      <c r="A24" t="n" s="486">
         <v>2011.0</v>
       </c>
-      <c r="B24" t="n" s="219">
+      <c r="B24" t="n" s="521">
         <v>0.5229974125</v>
       </c>
-      <c r="C24" t="n" s="253">
+      <c r="C24" t="n" s="555">
         <v>4803.601000000001</v>
       </c>
-      <c r="D24" t="n" s="288">
+      <c r="D24" t="n" s="590">
         <v>6214.8155</v>
       </c>
       <c r="E24"/>
     </row>
     <row r="25">
-      <c r="A25" t="n" s="185">
+      <c r="A25" t="n" s="487">
         <v>2012.0</v>
       </c>
-      <c r="B25" t="n" s="220">
+      <c r="B25" t="n" s="522">
         <v>0.29177867175</v>
       </c>
-      <c r="C25" t="n" s="254">
+      <c r="C25" t="n" s="556">
         <v>4187.97</v>
       </c>
-      <c r="D25" t="n" s="289">
+      <c r="D25" t="n" s="591">
         <v>3517.691754471992</v>
       </c>
       <c r="E25"/>
     </row>
     <row r="26">
-      <c r="A26" t="n" s="186">
+      <c r="A26" t="n" s="488">
         <v>2013.0</v>
       </c>
-      <c r="B26" t="n" s="221">
+      <c r="B26" t="n" s="523">
         <v>1.1386274275</v>
       </c>
-      <c r="C26" t="n" s="255">
+      <c r="C26" t="n" s="557">
         <v>5325.24</v>
       </c>
-      <c r="D26" t="n" s="290">
+      <c r="D26" t="n" s="592">
         <v>8267.3174</v>
       </c>
       <c r="E26"/>
     </row>
     <row r="27">
-      <c r="A27" t="n" s="187">
+      <c r="A27" t="n" s="489">
         <v>2014.0</v>
       </c>
-      <c r="B27" t="n" s="222">
+      <c r="B27" t="n" s="524">
         <v>0.96979492825</v>
       </c>
-      <c r="C27" t="n" s="256">
+      <c r="C27" t="n" s="558">
         <v>3824.0060000000003</v>
       </c>
-      <c r="D27" t="n" s="291">
+      <c r="D27" t="n" s="593">
         <v>7467.039400000001</v>
       </c>
-      <c r="E27" t="n" s="300">
+      <c r="E27" t="n" s="602">
         <v>167.023</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n" s="188">
+      <c r="A28" t="n" s="490">
         <v>2015.0</v>
       </c>
-      <c r="B28" t="n" s="223">
+      <c r="B28" t="n" s="525">
         <v>0.7373811</v>
       </c>
-      <c r="C28" t="n" s="257">
+      <c r="C28" t="n" s="559">
         <v>2415.722</v>
       </c>
-      <c r="D28" t="n" s="292">
+      <c r="D28" t="n" s="594">
         <v>6580.7147</v>
       </c>
-      <c r="E28" t="n" s="301">
+      <c r="E28" t="n" s="603">
         <v>93.231</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n" s="189">
+      <c r="A29" t="n" s="491">
         <v>2016.0</v>
       </c>
-      <c r="B29" t="n" s="224">
+      <c r="B29" t="n" s="526">
         <v>0.8860630349999999</v>
       </c>
-      <c r="C29" t="n" s="258">
+      <c r="C29" t="n" s="560">
         <v>4058.169</v>
       </c>
-      <c r="D29" t="n" s="293">
+      <c r="D29" t="n" s="595">
         <v>6204.9642</v>
       </c>
-      <c r="E29" t="n" s="302">
+      <c r="E29" t="n" s="604">
         <v>181.573</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n" s="190">
+      <c r="A30" t="n" s="492">
         <v>2017.0</v>
       </c>
-      <c r="B30" t="n" s="225">
+      <c r="B30" t="n" s="527">
         <v>0.9481421505000001</v>
       </c>
-      <c r="C30" t="n" s="259">
+      <c r="C30" t="n" s="561">
         <v>2319.732</v>
       </c>
-      <c r="D30" t="n" s="294">
+      <c r="D30" t="n" s="596">
         <v>3787.9462000000003</v>
       </c>
-      <c r="E30" t="n" s="303">
+      <c r="E30" t="n" s="605">
         <v>186.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n" s="191">
+      <c r="A31" t="n" s="493">
         <v>2018.0</v>
       </c>
-      <c r="B31" t="n" s="226">
+      <c r="B31" t="n" s="528">
         <v>0.51483839075</v>
       </c>
-      <c r="C31" t="n" s="260">
+      <c r="C31" t="n" s="562">
         <v>2188.357</v>
       </c>
-      <c r="D31" t="n" s="295">
+      <c r="D31" t="n" s="597">
         <v>3663.6322999999998</v>
       </c>
-      <c r="E31" t="n" s="304">
+      <c r="E31" t="n" s="606">
         <v>151.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n" s="192">
+      <c r="A32" t="n" s="494">
         <v>2019.0</v>
       </c>
-      <c r="B32" t="n" s="227">
+      <c r="B32" t="n" s="529">
         <v>0.546739615</v>
       </c>
-      <c r="C32" t="n" s="261">
+      <c r="C32" t="n" s="563">
         <v>4878.317</v>
       </c>
-      <c r="D32" t="n" s="296">
+      <c r="D32" t="n" s="598">
         <v>6384.7071</v>
       </c>
-      <c r="E32" t="n" s="305">
+      <c r="E32" t="n" s="607">
         <v>87.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n" s="193">
+      <c r="A33" t="n" s="495">
         <v>2020.0</v>
       </c>
-      <c r="B33" t="n" s="228">
+      <c r="B33" t="n" s="530">
         <v>0.802187205</v>
       </c>
-      <c r="C33" t="n" s="262">
+      <c r="C33" t="n" s="564">
         <v>5568.857</v>
       </c>
-      <c r="D33" t="n" s="297">
+      <c r="D33" t="n" s="599">
         <v>7739.671200000001</v>
       </c>
-      <c r="E33" t="n" s="306">
+      <c r="E33" t="n" s="608">
         <v>121.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n" s="194">
+      <c r="A34" t="n" s="496">
         <v>2021.0</v>
       </c>
-      <c r="B34" t="n" s="229">
+      <c r="B34" t="n" s="531">
         <v>0.8022234775</v>
       </c>
-      <c r="C34" t="n" s="263">
+      <c r="C34" t="n" s="565">
         <v>3509.97</v>
       </c>
-      <c r="D34" t="n" s="298">
+      <c r="D34" t="n" s="600">
         <v>6499.268999999999</v>
       </c>
-      <c r="E34" t="n" s="307">
+      <c r="E34" t="n" s="609">
         <v>132.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n" s="195">
+      <c r="A35" t="n" s="497">
         <v>2022.0</v>
       </c>
-      <c r="B35" t="n" s="230">
+      <c r="B35" t="n" s="532">
         <v>0.8699506025</v>
       </c>
-      <c r="C35" t="n" s="264">
+      <c r="C35" t="n" s="566">
         <v>5594.4400000000005</v>
       </c>
-      <c r="D35" t="n" s="299">
+      <c r="D35" t="n" s="601">
         <v>7043.8695317</v>
       </c>
       <c r="E35"/>
     </row>
     <row r="36">
-      <c r="A36" t="n" s="196">
+      <c r="A36" t="n" s="498">
         <v>2023.0</v>
       </c>
       <c r="B36"/>
-      <c r="C36" t="n" s="265">
+      <c r="C36" t="n" s="567">
         <v>2226.324</v>
       </c>
       <c r="D36"/>

</xml_diff>

<commit_message>
Run with the comparison plot and correction of the caption of that figure
</commit_message>
<xml_diff>
--- a/results/2023_Summaryplots.xlsx
+++ b/results/2023_Summaryplots.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -88,13 +88,919 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="308">
+  <cellXfs count="610">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
       <alignment wrapText="true"/>
     </xf>
@@ -1022,554 +1928,554 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="157">
+      <c r="A1" t="s" s="459">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="158">
+      <c r="B1" t="s" s="460">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="159">
+      <c r="C1" t="s" s="461">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="160">
+      <c r="D1" t="s" s="462">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="161">
+      <c r="E1" t="s" s="463">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="162">
+      <c r="A2" t="n" s="464">
         <v>1989.0</v>
       </c>
-      <c r="B2" t="n" s="197">
+      <c r="B2" t="n" s="499">
         <v>0.4855439795</v>
       </c>
-      <c r="C2" t="n" s="231">
+      <c r="C2" t="n" s="533">
         <v>4738.96</v>
       </c>
-      <c r="D2" t="n" s="266">
+      <c r="D2" t="n" s="568">
         <v>5319.032</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="163">
+      <c r="A3" t="n" s="465">
         <v>1990.0</v>
       </c>
-      <c r="B3" t="n" s="198">
+      <c r="B3" t="n" s="500">
         <v>1.5074486125</v>
       </c>
-      <c r="C3" t="n" s="232">
+      <c r="C3" t="n" s="534">
         <v>5821.553</v>
       </c>
-      <c r="D3" t="n" s="267">
+      <c r="D3" t="n" s="569">
         <v>6689.548000000001</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="164">
+      <c r="A4" t="n" s="466">
         <v>1991.0</v>
       </c>
-      <c r="B4" t="n" s="199">
+      <c r="B4" t="n" s="501">
         <v>0.6125907275</v>
       </c>
-      <c r="C4" t="n" s="233">
+      <c r="C4" t="n" s="535">
         <v>2867.163</v>
       </c>
-      <c r="D4" t="n" s="268">
+      <c r="D4" t="n" s="570">
         <v>3468.7690000000002</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="165">
+      <c r="A5" t="n" s="467">
         <v>1992.0</v>
       </c>
-      <c r="B5" t="n" s="200">
+      <c r="B5" t="n" s="502">
         <v>0.39766832315</v>
       </c>
-      <c r="C5" t="n" s="234">
+      <c r="C5" t="n" s="536">
         <v>2903.2619999999997</v>
       </c>
-      <c r="D5" t="n" s="269">
+      <c r="D5" t="n" s="571">
         <v>2191.456</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="166">
+      <c r="A6" t="n" s="468">
         <v>1993.0</v>
       </c>
-      <c r="B6" t="n" s="201">
+      <c r="B6" t="n" s="503">
         <v>1.0468879075</v>
       </c>
-      <c r="C6" t="n" s="235">
+      <c r="C6" t="n" s="537">
         <v>3074.6600000000003</v>
       </c>
-      <c r="D6" t="n" s="270">
+      <c r="D6" t="n" s="572">
         <v>3016.8668</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="167">
+      <c r="A7" t="n" s="469">
         <v>1994.0</v>
       </c>
-      <c r="B7" t="n" s="202">
+      <c r="B7" t="n" s="504">
         <v>0.0930753435</v>
       </c>
-      <c r="C7" t="n" s="236">
+      <c r="C7" t="n" s="538">
         <v>1733.716</v>
       </c>
-      <c r="D7" t="n" s="271">
+      <c r="D7" t="n" s="573">
         <v>555.76974</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="168">
+      <c r="A8" t="n" s="470">
         <v>1995.0</v>
       </c>
-      <c r="B8" t="n" s="203">
+      <c r="B8" t="n" s="505">
         <v>0.13298446849999998</v>
       </c>
-      <c r="C8" t="n" s="237">
+      <c r="C8" t="n" s="539">
         <v>5764.99</v>
       </c>
-      <c r="D8" t="n" s="272">
+      <c r="D8" t="n" s="574">
         <v>1153.59391</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="169">
+      <c r="A9" t="n" s="471">
         <v>1996.0</v>
       </c>
-      <c r="B9" t="n" s="204">
+      <c r="B9" t="n" s="506">
         <v>0.6267725125</v>
       </c>
-      <c r="C9" t="n" s="238">
+      <c r="C9" t="n" s="540">
         <v>13102.27</v>
       </c>
-      <c r="D9" t="n" s="273">
+      <c r="D9" t="n" s="575">
         <v>3001.0653</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="170">
+      <c r="A10" t="n" s="472">
         <v>1997.0</v>
       </c>
-      <c r="B10" t="n" s="205">
+      <c r="B10" t="n" s="507">
         <v>0.86079134</v>
       </c>
-      <c r="C10" t="n" s="239">
+      <c r="C10" t="n" s="541">
         <v>10267.76</v>
       </c>
-      <c r="D10" t="n" s="274">
+      <c r="D10" t="n" s="576">
         <v>6552.2829</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="171">
+      <c r="A11" t="n" s="473">
         <v>1998.0</v>
       </c>
-      <c r="B11" t="n" s="206">
+      <c r="B11" t="n" s="508">
         <v>1.6326542475</v>
       </c>
-      <c r="C11" t="n" s="240">
+      <c r="C11" t="n" s="542">
         <v>9592.050000000001</v>
       </c>
-      <c r="D11" t="n" s="275">
+      <c r="D11" t="n" s="577">
         <v>9258.5939</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="172">
+      <c r="A12" t="n" s="474">
         <v>1999.0</v>
       </c>
-      <c r="B12" t="n" s="207">
+      <c r="B12" t="n" s="509">
         <v>0.77140627</v>
       </c>
-      <c r="C12" t="n" s="241">
+      <c r="C12" t="n" s="543">
         <v>3667.5890000000004</v>
       </c>
-      <c r="D12" t="n" s="276">
+      <c r="D12" t="n" s="578">
         <v>3387.3143</v>
       </c>
       <c r="E12"/>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="173">
+      <c r="A13" t="n" s="475">
         <v>2000.0</v>
       </c>
-      <c r="B13" t="n" s="208">
+      <c r="B13" t="n" s="510">
         <v>0.5941586025</v>
       </c>
-      <c r="C13" t="n" s="242">
+      <c r="C13" t="n" s="544">
         <v>4735.55</v>
       </c>
-      <c r="D13" t="n" s="277">
+      <c r="D13" t="n" s="579">
         <v>5545.81998</v>
       </c>
       <c r="E13"/>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="174">
+      <c r="A14" t="n" s="476">
         <v>2001.0</v>
       </c>
-      <c r="B14" t="n" s="209">
+      <c r="B14" t="n" s="511">
         <v>0.88446172</v>
       </c>
-      <c r="C14" t="n" s="243">
+      <c r="C14" t="n" s="545">
         <v>7978.05</v>
       </c>
-      <c r="D14" t="n" s="278">
+      <c r="D14" t="n" s="580">
         <v>9093.53857</v>
       </c>
       <c r="E14"/>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="175">
+      <c r="A15" t="n" s="477">
         <v>2002.0</v>
       </c>
-      <c r="B15" t="n" s="210">
+      <c r="B15" t="n" s="512">
         <v>0.740033745</v>
       </c>
-      <c r="C15" t="n" s="244">
+      <c r="C15" t="n" s="546">
         <v>6343.438</v>
       </c>
-      <c r="D15" t="n" s="279">
+      <c r="D15" t="n" s="581">
         <v>7081.3061800000005</v>
       </c>
       <c r="E15"/>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="176">
+      <c r="A16" t="n" s="478">
         <v>2003.0</v>
       </c>
-      <c r="B16" t="n" s="211">
+      <c r="B16" t="n" s="513">
         <v>0.7464939675</v>
       </c>
-      <c r="C16" t="n" s="245">
+      <c r="C16" t="n" s="547">
         <v>3440.3100000000004</v>
       </c>
-      <c r="D16" t="n" s="280">
+      <c r="D16" t="n" s="582">
         <v>4742.13649</v>
       </c>
       <c r="E16"/>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="177">
+      <c r="A17" t="n" s="479">
         <v>2004.0</v>
       </c>
-      <c r="B17" t="n" s="212">
+      <c r="B17" t="n" s="514">
         <v>1.05968224</v>
       </c>
-      <c r="C17" t="n" s="246">
+      <c r="C17" t="n" s="548">
         <v>2637.61</v>
       </c>
-      <c r="D17" t="n" s="281">
+      <c r="D17" t="n" s="583">
         <v>5871.08189</v>
       </c>
       <c r="E17"/>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="178">
+      <c r="A18" t="n" s="480">
         <v>2005.0</v>
       </c>
-      <c r="B18" t="n" s="213">
+      <c r="B18" t="n" s="515">
         <v>0.5298815047500001</v>
       </c>
-      <c r="C18" t="n" s="247">
+      <c r="C18" t="n" s="549">
         <v>2410.866</v>
       </c>
-      <c r="D18" t="n" s="282">
+      <c r="D18" t="n" s="584">
         <v>4744.4489</v>
       </c>
       <c r="E18"/>
     </row>
     <row r="19">
-      <c r="A19" t="n" s="179">
+      <c r="A19" t="n" s="481">
         <v>2006.0</v>
       </c>
-      <c r="B19" t="n" s="214">
+      <c r="B19" t="n" s="516">
         <v>0.441407338</v>
       </c>
-      <c r="C19" t="n" s="248">
+      <c r="C19" t="n" s="550">
         <v>4231.9490000000005</v>
       </c>
-      <c r="D19" t="n" s="283">
+      <c r="D19" t="n" s="585">
         <v>4267.4956999999995</v>
       </c>
       <c r="E19"/>
     </row>
     <row r="20">
-      <c r="A20" t="n" s="180">
+      <c r="A20" t="n" s="482">
         <v>2007.0</v>
       </c>
-      <c r="B20" t="n" s="215">
+      <c r="B20" t="n" s="517">
         <v>0.511637735</v>
       </c>
-      <c r="C20" t="n" s="249">
+      <c r="C20" t="n" s="551">
         <v>6271.51</v>
       </c>
-      <c r="D20" t="n" s="284">
+      <c r="D20" t="n" s="586">
         <v>3517.3119</v>
       </c>
       <c r="E20"/>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="181">
+      <c r="A21" t="n" s="483">
         <v>2008.0</v>
       </c>
-      <c r="B21" t="n" s="216">
+      <c r="B21" t="n" s="518">
         <v>0.831230995</v>
       </c>
-      <c r="C21" t="n" s="250">
+      <c r="C21" t="n" s="552">
         <v>3749.02</v>
       </c>
-      <c r="D21" t="n" s="285">
+      <c r="D21" t="n" s="587">
         <v>3299.5126</v>
       </c>
       <c r="E21"/>
     </row>
     <row r="22">
-      <c r="A22" t="n" s="182">
+      <c r="A22" t="n" s="484">
         <v>2009.0</v>
       </c>
-      <c r="B22" t="n" s="217">
+      <c r="B22" t="n" s="519">
         <v>1.1888285455</v>
       </c>
-      <c r="C22" t="n" s="251">
+      <c r="C22" t="n" s="553">
         <v>1471.57</v>
       </c>
-      <c r="D22" t="n" s="286">
+      <c r="D22" t="n" s="588">
         <v>2916.9067</v>
       </c>
       <c r="E22"/>
     </row>
     <row r="23">
-      <c r="A23" t="n" s="183">
+      <c r="A23" t="n" s="485">
         <v>2010.0</v>
       </c>
-      <c r="B23" t="n" s="218">
+      <c r="B23" t="n" s="520">
         <v>0.65105517</v>
       </c>
-      <c r="C23" t="n" s="252">
+      <c r="C23" t="n" s="554">
         <v>1226.134</v>
       </c>
-      <c r="D23" t="n" s="287">
+      <c r="D23" t="n" s="589">
         <v>4820.6776</v>
       </c>
       <c r="E23"/>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="184">
+      <c r="A24" t="n" s="486">
         <v>2011.0</v>
       </c>
-      <c r="B24" t="n" s="219">
+      <c r="B24" t="n" s="521">
         <v>0.6865381875000001</v>
       </c>
-      <c r="C24" t="n" s="253">
+      <c r="C24" t="n" s="555">
         <v>3671.896</v>
       </c>
-      <c r="D24" t="n" s="288">
+      <c r="D24" t="n" s="590">
         <v>6214.8155</v>
       </c>
       <c r="E24"/>
     </row>
     <row r="25">
-      <c r="A25" t="n" s="185">
+      <c r="A25" t="n" s="487">
         <v>2012.0</v>
       </c>
-      <c r="B25" t="n" s="220">
+      <c r="B25" t="n" s="522">
         <v>0.4991767475</v>
       </c>
-      <c r="C25" t="n" s="254">
+      <c r="C25" t="n" s="556">
         <v>3310.95</v>
       </c>
-      <c r="D25" t="n" s="289">
+      <c r="D25" t="n" s="591">
         <v>3517.691754471992</v>
       </c>
       <c r="E25"/>
     </row>
     <row r="26">
-      <c r="A26" t="n" s="186">
+      <c r="A26" t="n" s="488">
         <v>2013.0</v>
       </c>
-      <c r="B26" t="n" s="221">
+      <c r="B26" t="n" s="523">
         <v>1.2880664025</v>
       </c>
-      <c r="C26" t="n" s="255">
+      <c r="C26" t="n" s="557">
         <v>5010.61</v>
       </c>
-      <c r="D26" t="n" s="290">
+      <c r="D26" t="n" s="592">
         <v>8267.3174</v>
       </c>
       <c r="E26"/>
     </row>
     <row r="27">
-      <c r="A27" t="n" s="187">
+      <c r="A27" t="n" s="489">
         <v>2014.0</v>
       </c>
-      <c r="B27" t="n" s="222">
+      <c r="B27" t="n" s="524">
         <v>0.96111820425</v>
       </c>
-      <c r="C27" t="n" s="256">
+      <c r="C27" t="n" s="558">
         <v>4003.25</v>
       </c>
-      <c r="D27" t="n" s="291">
+      <c r="D27" t="n" s="593">
         <v>7467.039400000001</v>
       </c>
-      <c r="E27" t="n" s="300">
+      <c r="E27" t="n" s="602">
         <v>167.023</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n" s="188">
+      <c r="A28" t="n" s="490">
         <v>2015.0</v>
       </c>
-      <c r="B28" t="n" s="223">
+      <c r="B28" t="n" s="525">
         <v>0.811322425</v>
       </c>
-      <c r="C28" t="n" s="257">
+      <c r="C28" t="n" s="559">
         <v>2293.468</v>
       </c>
-      <c r="D28" t="n" s="292">
+      <c r="D28" t="n" s="594">
         <v>6580.7147</v>
       </c>
-      <c r="E28" t="n" s="301">
+      <c r="E28" t="n" s="603">
         <v>93.231</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n" s="189">
+      <c r="A29" t="n" s="491">
         <v>2016.0</v>
       </c>
-      <c r="B29" t="n" s="224">
+      <c r="B29" t="n" s="526">
         <v>1.0855834500000001</v>
       </c>
-      <c r="C29" t="n" s="258">
+      <c r="C29" t="n" s="560">
         <v>2855.058</v>
       </c>
-      <c r="D29" t="n" s="293">
+      <c r="D29" t="n" s="595">
         <v>6204.9642</v>
       </c>
-      <c r="E29" t="n" s="302">
+      <c r="E29" t="n" s="604">
         <v>181.573</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n" s="190">
+      <c r="A30" t="n" s="492">
         <v>2017.0</v>
       </c>
-      <c r="B30" t="n" s="225">
+      <c r="B30" t="n" s="527">
         <v>1.144991095</v>
       </c>
-      <c r="C30" t="n" s="259">
+      <c r="C30" t="n" s="561">
         <v>1796.439</v>
       </c>
-      <c r="D30" t="n" s="294">
+      <c r="D30" t="n" s="596">
         <v>3787.9462000000003</v>
       </c>
-      <c r="E30" t="n" s="303">
+      <c r="E30" t="n" s="605">
         <v>186.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n" s="191">
+      <c r="A31" t="n" s="493">
         <v>2018.0</v>
       </c>
-      <c r="B31" t="n" s="226">
+      <c r="B31" t="n" s="528">
         <v>0.79383421025</v>
       </c>
-      <c r="C31" t="n" s="260">
+      <c r="C31" t="n" s="562">
         <v>1454.472</v>
       </c>
-      <c r="D31" t="n" s="295">
+      <c r="D31" t="n" s="597">
         <v>3663.6322999999998</v>
       </c>
-      <c r="E31" t="n" s="304">
+      <c r="E31" t="n" s="606">
         <v>151.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n" s="192">
+      <c r="A32" t="n" s="494">
         <v>2019.0</v>
       </c>
-      <c r="B32" t="n" s="227">
+      <c r="B32" t="n" s="529">
         <v>0.80834273</v>
       </c>
-      <c r="C32" t="n" s="261">
+      <c r="C32" t="n" s="563">
         <v>3298.122</v>
       </c>
-      <c r="D32" t="n" s="296">
+      <c r="D32" t="n" s="598">
         <v>6384.7071</v>
       </c>
-      <c r="E32" t="n" s="305">
+      <c r="E32" t="n" s="607">
         <v>87.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n" s="193">
+      <c r="A33" t="n" s="495">
         <v>2020.0</v>
       </c>
-      <c r="B33" t="n" s="228">
+      <c r="B33" t="n" s="530">
         <v>1.08246269</v>
       </c>
-      <c r="C33" t="n" s="262">
+      <c r="C33" t="n" s="564">
         <v>3951.592</v>
       </c>
-      <c r="D33" t="n" s="297">
+      <c r="D33" t="n" s="599">
         <v>7739.671200000001</v>
       </c>
-      <c r="E33" t="n" s="306">
+      <c r="E33" t="n" s="608">
         <v>121.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n" s="194">
+      <c r="A34" t="n" s="496">
         <v>2021.0</v>
       </c>
-      <c r="B34" t="n" s="229">
+      <c r="B34" t="n" s="531">
         <v>1.1311449975</v>
       </c>
-      <c r="C34" t="n" s="263">
+      <c r="C34" t="n" s="565">
         <v>3331.913</v>
       </c>
-      <c r="D34" t="n" s="298">
+      <c r="D34" t="n" s="600">
         <v>6499.268999999999</v>
       </c>
-      <c r="E34" t="n" s="307">
+      <c r="E34" t="n" s="609">
         <v>132.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n" s="195">
+      <c r="A35" t="n" s="497">
         <v>2022.0</v>
       </c>
-      <c r="B35" t="n" s="230">
+      <c r="B35" t="n" s="532">
         <v>1.0317264475</v>
       </c>
-      <c r="C35" t="n" s="264">
+      <c r="C35" t="n" s="566">
         <v>2593.236</v>
       </c>
-      <c r="D35" t="n" s="299">
+      <c r="D35" t="n" s="601">
         <v>7043.8695317</v>
       </c>
       <c r="E35"/>
     </row>
     <row r="36">
-      <c r="A36" t="n" s="196">
+      <c r="A36" t="n" s="498">
         <v>2023.0</v>
       </c>
       <c r="B36"/>
-      <c r="C36" t="n" s="265">
+      <c r="C36" t="n" s="567">
         <v>4402.420999999999</v>
       </c>
       <c r="D36"/>

</xml_diff>

<commit_message>
corrected caption figure 16
</commit_message>
<xml_diff>
--- a/results/2023_Summaryplots.xlsx
+++ b/results/2023_Summaryplots.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -88,13 +88,466 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="610">
+  <cellXfs count="761">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
       <alignment wrapText="true"/>
     </xf>
@@ -1928,554 +2381,554 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="459">
+      <c r="A1" t="s" s="610">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="460">
+      <c r="B1" t="s" s="611">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="461">
+      <c r="C1" t="s" s="612">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="462">
+      <c r="D1" t="s" s="613">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="463">
+      <c r="E1" t="s" s="614">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="464">
+      <c r="A2" t="n" s="615">
         <v>1989.0</v>
       </c>
-      <c r="B2" t="n" s="499">
+      <c r="B2" t="n" s="650">
         <v>0.4855439795</v>
       </c>
-      <c r="C2" t="n" s="533">
+      <c r="C2" t="n" s="684">
         <v>4738.96</v>
       </c>
-      <c r="D2" t="n" s="568">
+      <c r="D2" t="n" s="719">
         <v>5319.032</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="465">
+      <c r="A3" t="n" s="616">
         <v>1990.0</v>
       </c>
-      <c r="B3" t="n" s="500">
+      <c r="B3" t="n" s="651">
         <v>1.5074486125</v>
       </c>
-      <c r="C3" t="n" s="534">
+      <c r="C3" t="n" s="685">
         <v>5821.553</v>
       </c>
-      <c r="D3" t="n" s="569">
+      <c r="D3" t="n" s="720">
         <v>6689.548000000001</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="466">
+      <c r="A4" t="n" s="617">
         <v>1991.0</v>
       </c>
-      <c r="B4" t="n" s="501">
+      <c r="B4" t="n" s="652">
         <v>0.6125907275</v>
       </c>
-      <c r="C4" t="n" s="535">
+      <c r="C4" t="n" s="686">
         <v>2867.163</v>
       </c>
-      <c r="D4" t="n" s="570">
+      <c r="D4" t="n" s="721">
         <v>3468.7690000000002</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="467">
+      <c r="A5" t="n" s="618">
         <v>1992.0</v>
       </c>
-      <c r="B5" t="n" s="502">
+      <c r="B5" t="n" s="653">
         <v>0.39766832315</v>
       </c>
-      <c r="C5" t="n" s="536">
+      <c r="C5" t="n" s="687">
         <v>2903.2619999999997</v>
       </c>
-      <c r="D5" t="n" s="571">
+      <c r="D5" t="n" s="722">
         <v>2191.456</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="468">
+      <c r="A6" t="n" s="619">
         <v>1993.0</v>
       </c>
-      <c r="B6" t="n" s="503">
+      <c r="B6" t="n" s="654">
         <v>1.0468879075</v>
       </c>
-      <c r="C6" t="n" s="537">
+      <c r="C6" t="n" s="688">
         <v>3074.6600000000003</v>
       </c>
-      <c r="D6" t="n" s="572">
+      <c r="D6" t="n" s="723">
         <v>3016.8668</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="469">
+      <c r="A7" t="n" s="620">
         <v>1994.0</v>
       </c>
-      <c r="B7" t="n" s="504">
+      <c r="B7" t="n" s="655">
         <v>0.0930753435</v>
       </c>
-      <c r="C7" t="n" s="538">
+      <c r="C7" t="n" s="689">
         <v>1733.716</v>
       </c>
-      <c r="D7" t="n" s="573">
+      <c r="D7" t="n" s="724">
         <v>555.76974</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="470">
+      <c r="A8" t="n" s="621">
         <v>1995.0</v>
       </c>
-      <c r="B8" t="n" s="505">
+      <c r="B8" t="n" s="656">
         <v>0.13298446849999998</v>
       </c>
-      <c r="C8" t="n" s="539">
+      <c r="C8" t="n" s="690">
         <v>5764.99</v>
       </c>
-      <c r="D8" t="n" s="574">
+      <c r="D8" t="n" s="725">
         <v>1153.59391</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="471">
+      <c r="A9" t="n" s="622">
         <v>1996.0</v>
       </c>
-      <c r="B9" t="n" s="506">
+      <c r="B9" t="n" s="657">
         <v>0.6267725125</v>
       </c>
-      <c r="C9" t="n" s="540">
+      <c r="C9" t="n" s="691">
         <v>13102.27</v>
       </c>
-      <c r="D9" t="n" s="575">
+      <c r="D9" t="n" s="726">
         <v>3001.0653</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="472">
+      <c r="A10" t="n" s="623">
         <v>1997.0</v>
       </c>
-      <c r="B10" t="n" s="507">
+      <c r="B10" t="n" s="658">
         <v>0.86079134</v>
       </c>
-      <c r="C10" t="n" s="541">
+      <c r="C10" t="n" s="692">
         <v>10267.76</v>
       </c>
-      <c r="D10" t="n" s="576">
+      <c r="D10" t="n" s="727">
         <v>6552.2829</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="473">
+      <c r="A11" t="n" s="624">
         <v>1998.0</v>
       </c>
-      <c r="B11" t="n" s="508">
+      <c r="B11" t="n" s="659">
         <v>1.6326542475</v>
       </c>
-      <c r="C11" t="n" s="542">
+      <c r="C11" t="n" s="693">
         <v>9592.050000000001</v>
       </c>
-      <c r="D11" t="n" s="577">
+      <c r="D11" t="n" s="728">
         <v>9258.5939</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="474">
+      <c r="A12" t="n" s="625">
         <v>1999.0</v>
       </c>
-      <c r="B12" t="n" s="509">
+      <c r="B12" t="n" s="660">
         <v>0.77140627</v>
       </c>
-      <c r="C12" t="n" s="543">
+      <c r="C12" t="n" s="694">
         <v>3667.5890000000004</v>
       </c>
-      <c r="D12" t="n" s="578">
+      <c r="D12" t="n" s="729">
         <v>3387.3143</v>
       </c>
       <c r="E12"/>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="475">
+      <c r="A13" t="n" s="626">
         <v>2000.0</v>
       </c>
-      <c r="B13" t="n" s="510">
+      <c r="B13" t="n" s="661">
         <v>0.5941586025</v>
       </c>
-      <c r="C13" t="n" s="544">
+      <c r="C13" t="n" s="695">
         <v>4735.55</v>
       </c>
-      <c r="D13" t="n" s="579">
+      <c r="D13" t="n" s="730">
         <v>5545.81998</v>
       </c>
       <c r="E13"/>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="476">
+      <c r="A14" t="n" s="627">
         <v>2001.0</v>
       </c>
-      <c r="B14" t="n" s="511">
+      <c r="B14" t="n" s="662">
         <v>0.88446172</v>
       </c>
-      <c r="C14" t="n" s="545">
+      <c r="C14" t="n" s="696">
         <v>7978.05</v>
       </c>
-      <c r="D14" t="n" s="580">
+      <c r="D14" t="n" s="731">
         <v>9093.53857</v>
       </c>
       <c r="E14"/>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="477">
+      <c r="A15" t="n" s="628">
         <v>2002.0</v>
       </c>
-      <c r="B15" t="n" s="512">
+      <c r="B15" t="n" s="663">
         <v>0.740033745</v>
       </c>
-      <c r="C15" t="n" s="546">
+      <c r="C15" t="n" s="697">
         <v>6343.438</v>
       </c>
-      <c r="D15" t="n" s="581">
+      <c r="D15" t="n" s="732">
         <v>7081.3061800000005</v>
       </c>
       <c r="E15"/>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="478">
+      <c r="A16" t="n" s="629">
         <v>2003.0</v>
       </c>
-      <c r="B16" t="n" s="513">
+      <c r="B16" t="n" s="664">
         <v>0.7464939675</v>
       </c>
-      <c r="C16" t="n" s="547">
+      <c r="C16" t="n" s="698">
         <v>3440.3100000000004</v>
       </c>
-      <c r="D16" t="n" s="582">
+      <c r="D16" t="n" s="733">
         <v>4742.13649</v>
       </c>
       <c r="E16"/>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="479">
+      <c r="A17" t="n" s="630">
         <v>2004.0</v>
       </c>
-      <c r="B17" t="n" s="514">
+      <c r="B17" t="n" s="665">
         <v>1.05968224</v>
       </c>
-      <c r="C17" t="n" s="548">
+      <c r="C17" t="n" s="699">
         <v>2637.61</v>
       </c>
-      <c r="D17" t="n" s="583">
+      <c r="D17" t="n" s="734">
         <v>5871.08189</v>
       </c>
       <c r="E17"/>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="480">
+      <c r="A18" t="n" s="631">
         <v>2005.0</v>
       </c>
-      <c r="B18" t="n" s="515">
+      <c r="B18" t="n" s="666">
         <v>0.5298815047500001</v>
       </c>
-      <c r="C18" t="n" s="549">
+      <c r="C18" t="n" s="700">
         <v>2410.866</v>
       </c>
-      <c r="D18" t="n" s="584">
+      <c r="D18" t="n" s="735">
         <v>4744.4489</v>
       </c>
       <c r="E18"/>
     </row>
     <row r="19">
-      <c r="A19" t="n" s="481">
+      <c r="A19" t="n" s="632">
         <v>2006.0</v>
       </c>
-      <c r="B19" t="n" s="516">
+      <c r="B19" t="n" s="667">
         <v>0.441407338</v>
       </c>
-      <c r="C19" t="n" s="550">
+      <c r="C19" t="n" s="701">
         <v>4231.9490000000005</v>
       </c>
-      <c r="D19" t="n" s="585">
+      <c r="D19" t="n" s="736">
         <v>4267.4956999999995</v>
       </c>
       <c r="E19"/>
     </row>
     <row r="20">
-      <c r="A20" t="n" s="482">
+      <c r="A20" t="n" s="633">
         <v>2007.0</v>
       </c>
-      <c r="B20" t="n" s="517">
+      <c r="B20" t="n" s="668">
         <v>0.511637735</v>
       </c>
-      <c r="C20" t="n" s="551">
+      <c r="C20" t="n" s="702">
         <v>6271.51</v>
       </c>
-      <c r="D20" t="n" s="586">
+      <c r="D20" t="n" s="737">
         <v>3517.3119</v>
       </c>
       <c r="E20"/>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="483">
+      <c r="A21" t="n" s="634">
         <v>2008.0</v>
       </c>
-      <c r="B21" t="n" s="518">
+      <c r="B21" t="n" s="669">
         <v>0.831230995</v>
       </c>
-      <c r="C21" t="n" s="552">
+      <c r="C21" t="n" s="703">
         <v>3749.02</v>
       </c>
-      <c r="D21" t="n" s="587">
+      <c r="D21" t="n" s="738">
         <v>3299.5126</v>
       </c>
       <c r="E21"/>
     </row>
     <row r="22">
-      <c r="A22" t="n" s="484">
+      <c r="A22" t="n" s="635">
         <v>2009.0</v>
       </c>
-      <c r="B22" t="n" s="519">
+      <c r="B22" t="n" s="670">
         <v>1.1888285455</v>
       </c>
-      <c r="C22" t="n" s="553">
+      <c r="C22" t="n" s="704">
         <v>1471.57</v>
       </c>
-      <c r="D22" t="n" s="588">
+      <c r="D22" t="n" s="739">
         <v>2916.9067</v>
       </c>
       <c r="E22"/>
     </row>
     <row r="23">
-      <c r="A23" t="n" s="485">
+      <c r="A23" t="n" s="636">
         <v>2010.0</v>
       </c>
-      <c r="B23" t="n" s="520">
+      <c r="B23" t="n" s="671">
         <v>0.65105517</v>
       </c>
-      <c r="C23" t="n" s="554">
+      <c r="C23" t="n" s="705">
         <v>1226.134</v>
       </c>
-      <c r="D23" t="n" s="589">
+      <c r="D23" t="n" s="740">
         <v>4820.6776</v>
       </c>
       <c r="E23"/>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="486">
+      <c r="A24" t="n" s="637">
         <v>2011.0</v>
       </c>
-      <c r="B24" t="n" s="521">
+      <c r="B24" t="n" s="672">
         <v>0.6865381875000001</v>
       </c>
-      <c r="C24" t="n" s="555">
+      <c r="C24" t="n" s="706">
         <v>3671.896</v>
       </c>
-      <c r="D24" t="n" s="590">
+      <c r="D24" t="n" s="741">
         <v>6214.8155</v>
       </c>
       <c r="E24"/>
     </row>
     <row r="25">
-      <c r="A25" t="n" s="487">
+      <c r="A25" t="n" s="638">
         <v>2012.0</v>
       </c>
-      <c r="B25" t="n" s="522">
+      <c r="B25" t="n" s="673">
         <v>0.4991767475</v>
       </c>
-      <c r="C25" t="n" s="556">
+      <c r="C25" t="n" s="707">
         <v>3310.95</v>
       </c>
-      <c r="D25" t="n" s="591">
+      <c r="D25" t="n" s="742">
         <v>3517.691754471992</v>
       </c>
       <c r="E25"/>
     </row>
     <row r="26">
-      <c r="A26" t="n" s="488">
+      <c r="A26" t="n" s="639">
         <v>2013.0</v>
       </c>
-      <c r="B26" t="n" s="523">
+      <c r="B26" t="n" s="674">
         <v>1.2880664025</v>
       </c>
-      <c r="C26" t="n" s="557">
+      <c r="C26" t="n" s="708">
         <v>5010.61</v>
       </c>
-      <c r="D26" t="n" s="592">
+      <c r="D26" t="n" s="743">
         <v>8267.3174</v>
       </c>
       <c r="E26"/>
     </row>
     <row r="27">
-      <c r="A27" t="n" s="489">
+      <c r="A27" t="n" s="640">
         <v>2014.0</v>
       </c>
-      <c r="B27" t="n" s="524">
+      <c r="B27" t="n" s="675">
         <v>0.96111820425</v>
       </c>
-      <c r="C27" t="n" s="558">
+      <c r="C27" t="n" s="709">
         <v>4003.25</v>
       </c>
-      <c r="D27" t="n" s="593">
+      <c r="D27" t="n" s="744">
         <v>7467.039400000001</v>
       </c>
-      <c r="E27" t="n" s="602">
+      <c r="E27" t="n" s="753">
         <v>167.023</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n" s="490">
+      <c r="A28" t="n" s="641">
         <v>2015.0</v>
       </c>
-      <c r="B28" t="n" s="525">
+      <c r="B28" t="n" s="676">
         <v>0.811322425</v>
       </c>
-      <c r="C28" t="n" s="559">
+      <c r="C28" t="n" s="710">
         <v>2293.468</v>
       </c>
-      <c r="D28" t="n" s="594">
+      <c r="D28" t="n" s="745">
         <v>6580.7147</v>
       </c>
-      <c r="E28" t="n" s="603">
+      <c r="E28" t="n" s="754">
         <v>93.231</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n" s="491">
+      <c r="A29" t="n" s="642">
         <v>2016.0</v>
       </c>
-      <c r="B29" t="n" s="526">
+      <c r="B29" t="n" s="677">
         <v>1.0855834500000001</v>
       </c>
-      <c r="C29" t="n" s="560">
+      <c r="C29" t="n" s="711">
         <v>2855.058</v>
       </c>
-      <c r="D29" t="n" s="595">
+      <c r="D29" t="n" s="746">
         <v>6204.9642</v>
       </c>
-      <c r="E29" t="n" s="604">
+      <c r="E29" t="n" s="755">
         <v>181.573</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n" s="492">
+      <c r="A30" t="n" s="643">
         <v>2017.0</v>
       </c>
-      <c r="B30" t="n" s="527">
+      <c r="B30" t="n" s="678">
         <v>1.144991095</v>
       </c>
-      <c r="C30" t="n" s="561">
+      <c r="C30" t="n" s="712">
         <v>1796.439</v>
       </c>
-      <c r="D30" t="n" s="596">
+      <c r="D30" t="n" s="747">
         <v>3787.9462000000003</v>
       </c>
-      <c r="E30" t="n" s="605">
+      <c r="E30" t="n" s="756">
         <v>186.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n" s="493">
+      <c r="A31" t="n" s="644">
         <v>2018.0</v>
       </c>
-      <c r="B31" t="n" s="528">
+      <c r="B31" t="n" s="679">
         <v>0.79383421025</v>
       </c>
-      <c r="C31" t="n" s="562">
+      <c r="C31" t="n" s="713">
         <v>1454.472</v>
       </c>
-      <c r="D31" t="n" s="597">
+      <c r="D31" t="n" s="748">
         <v>3663.6322999999998</v>
       </c>
-      <c r="E31" t="n" s="606">
+      <c r="E31" t="n" s="757">
         <v>151.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n" s="494">
+      <c r="A32" t="n" s="645">
         <v>2019.0</v>
       </c>
-      <c r="B32" t="n" s="529">
+      <c r="B32" t="n" s="680">
         <v>0.80834273</v>
       </c>
-      <c r="C32" t="n" s="563">
+      <c r="C32" t="n" s="714">
         <v>3298.122</v>
       </c>
-      <c r="D32" t="n" s="598">
+      <c r="D32" t="n" s="749">
         <v>6384.7071</v>
       </c>
-      <c r="E32" t="n" s="607">
+      <c r="E32" t="n" s="758">
         <v>87.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n" s="495">
+      <c r="A33" t="n" s="646">
         <v>2020.0</v>
       </c>
-      <c r="B33" t="n" s="530">
+      <c r="B33" t="n" s="681">
         <v>1.08246269</v>
       </c>
-      <c r="C33" t="n" s="564">
+      <c r="C33" t="n" s="715">
         <v>3951.592</v>
       </c>
-      <c r="D33" t="n" s="599">
+      <c r="D33" t="n" s="750">
         <v>7739.671200000001</v>
       </c>
-      <c r="E33" t="n" s="608">
+      <c r="E33" t="n" s="759">
         <v>121.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n" s="496">
+      <c r="A34" t="n" s="647">
         <v>2021.0</v>
       </c>
-      <c r="B34" t="n" s="531">
+      <c r="B34" t="n" s="682">
         <v>1.1311449975</v>
       </c>
-      <c r="C34" t="n" s="565">
+      <c r="C34" t="n" s="716">
         <v>3331.913</v>
       </c>
-      <c r="D34" t="n" s="600">
+      <c r="D34" t="n" s="751">
         <v>6499.268999999999</v>
       </c>
-      <c r="E34" t="n" s="609">
+      <c r="E34" t="n" s="760">
         <v>132.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n" s="497">
+      <c r="A35" t="n" s="648">
         <v>2022.0</v>
       </c>
-      <c r="B35" t="n" s="532">
+      <c r="B35" t="n" s="683">
         <v>1.0317264475</v>
       </c>
-      <c r="C35" t="n" s="566">
+      <c r="C35" t="n" s="717">
         <v>2593.236</v>
       </c>
-      <c r="D35" t="n" s="601">
+      <c r="D35" t="n" s="752">
         <v>7043.8695317</v>
       </c>
       <c r="E35"/>
     </row>
     <row r="36">
-      <c r="A36" t="n" s="498">
+      <c r="A36" t="n" s="649">
         <v>2023.0</v>
       </c>
       <c r="B36"/>
-      <c r="C36" t="n" s="567">
+      <c r="C36" t="n" s="718">
         <v>4402.420999999999</v>
       </c>
       <c r="D36"/>

</xml_diff>